<commit_message>
Refactor chemicalList and sectionList scripts to improve data handling and update column titles
</commit_message>
<xml_diff>
--- a/assets/file/template/Chemical list.xlsx
+++ b/assets/file/template/Chemical list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\amecnas\amecweb\wwwroot\development\safety\assets\file\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docker\src\safety\assets\file\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672E4B3-735F-4B53-9CC7-615896B35501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9067CD79-857E-4998-A9F3-AFA332778ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>MANUFACTURER / VENDOR</t>
   </si>
   <si>
-    <t>UN CLASS</t>
-  </si>
-  <si>
     <t>Rev.</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   <si>
     <t>PUR.
 INCHARGE</t>
+  </si>
+  <si>
+    <t>CLASS</t>
   </si>
 </sst>
 </file>
@@ -563,18 +563,18 @@
   <dimension ref="A1:BC15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="3.75" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="7" customWidth="1"/>
-    <col min="2" max="4" width="14.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="7" customWidth="1"/>
-    <col min="6" max="7" width="43.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="7" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="3.7109375" style="7"/>
+    <col min="1" max="1" width="5.75" style="7" customWidth="1"/>
+    <col min="2" max="4" width="14.75" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16.75" style="7" customWidth="1"/>
+    <col min="6" max="7" width="43.75" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.75" style="7" customWidth="1"/>
+    <col min="9" max="10" width="9.125" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="3.75" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.65">
@@ -587,16 +587,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>2</v>
@@ -605,13 +605,13 @@
         <v>3</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -727,7 +727,7 @@
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -736,10 +736,10 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -767,20 +767,20 @@
     <row r="11" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A11" s="11"/>
       <c r="B11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>10</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -808,20 +808,20 @@
     <row r="12" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A12" s="11"/>
       <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -849,20 +849,20 @@
     <row r="13" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A13" s="11"/>
       <c r="B13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -890,20 +890,20 @@
     <row r="14" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A14" s="11"/>
       <c r="B14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>

</xml_diff>